<commit_message>
updated the Analysis file
</commit_message>
<xml_diff>
--- a/NSFNET.xlsx
+++ b/NSFNET.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Proposed Model</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>CPU Utilization Ratio</t>
+  </si>
+  <si>
+    <t>Thesis</t>
   </si>
   <si>
     <t>Number of SFC Accepted</t>
@@ -86,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -110,6 +113,9 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
@@ -249,11 +255,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1689205209"/>
-        <c:axId val="1246122061"/>
+        <c:axId val="1054620654"/>
+        <c:axId val="844498453"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1689205209"/>
+        <c:axId val="1054620654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -305,10 +311,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1246122061"/>
+        <c:crossAx val="844498453"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1246122061"/>
+        <c:axId val="844498453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -385,7 +391,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1689205209"/>
+        <c:crossAx val="1054620654"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -501,11 +507,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1008293702"/>
-        <c:axId val="1545173196"/>
+        <c:axId val="863377582"/>
+        <c:axId val="583961850"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1008293702"/>
+        <c:axId val="863377582"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,10 +563,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1545173196"/>
+        <c:crossAx val="583961850"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1545173196"/>
+        <c:axId val="583961850"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,7 +641,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1008293702"/>
+        <c:crossAx val="863377582"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -662,6 +668,287 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="757575"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>CPU Utilisation Ratio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Proposed Model (on CNF)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4285F4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$72</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$2:$C$72</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Previous Model (on VNF)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="CC0000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="CC0000">
+                  <a:alpha val="100000"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="CC0000">
+                    <a:alpha val="100000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$72</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$72</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1633072072"/>
+        <c:axId val="16809466"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1633072072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Number of SFC Requests</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="16809466"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="16809466"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1633072072"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:title>
@@ -732,11 +1019,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1459438819"/>
-        <c:axId val="1750793849"/>
+        <c:axId val="1675736158"/>
+        <c:axId val="1281810282"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1459438819"/>
+        <c:axId val="1675736158"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,10 +1075,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1750793849"/>
+        <c:crossAx val="1281810282"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1750793849"/>
+        <c:axId val="1281810282"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -866,7 +1153,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1459438819"/>
+        <c:crossAx val="1675736158"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -926,10 +1213,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5591175" cy="3533775"/>
     <xdr:graphicFrame>
@@ -944,6 +1231,31 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5715000" cy="3619500"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -964,7 +1276,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3244,9 +3556,12 @@
       <c r="C1" s="9" t="s">
         <v>4</v>
       </c>
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="11">
         <v>70.0</v>
       </c>
       <c r="B2" s="4">
@@ -3256,9 +3571,12 @@
         <f t="shared" ref="C2:C72" si="1">B2/1400*100</f>
         <v>97.88238095</v>
       </c>
+      <c r="D2" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="11">
         <v>69.0</v>
       </c>
       <c r="B3" s="4">
@@ -3268,9 +3586,12 @@
         <f t="shared" si="1"/>
         <v>97.87238095</v>
       </c>
+      <c r="D3" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="11">
         <v>68.0</v>
       </c>
       <c r="B4" s="4">
@@ -3280,9 +3601,12 @@
         <f t="shared" si="1"/>
         <v>97.85238095</v>
       </c>
+      <c r="D4" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="10">
+      <c r="A5" s="11">
         <v>67.0</v>
       </c>
       <c r="B5" s="4">
@@ -3292,9 +3616,12 @@
         <f t="shared" si="1"/>
         <v>97.82238095</v>
       </c>
+      <c r="D5" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="10">
+      <c r="A6" s="11">
         <v>66.0</v>
       </c>
       <c r="B6" s="4">
@@ -3304,9 +3631,12 @@
         <f t="shared" si="1"/>
         <v>97.78238095</v>
       </c>
+      <c r="D6" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="10">
+      <c r="A7" s="11">
         <v>65.0</v>
       </c>
       <c r="B7" s="4">
@@ -3316,9 +3646,12 @@
         <f t="shared" si="1"/>
         <v>97.73238095</v>
       </c>
+      <c r="D7" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="10">
+      <c r="A8" s="11">
         <v>64.0</v>
       </c>
       <c r="B8" s="4">
@@ -3328,9 +3661,12 @@
         <f t="shared" si="1"/>
         <v>97.67238095</v>
       </c>
+      <c r="D8" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="10">
+      <c r="A9" s="11">
         <v>63.0</v>
       </c>
       <c r="B9" s="4">
@@ -3340,9 +3676,12 @@
         <f t="shared" si="1"/>
         <v>97.60238095</v>
       </c>
+      <c r="D9" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="10">
+      <c r="A10" s="11">
         <v>62.0</v>
       </c>
       <c r="B10" s="4">
@@ -3352,9 +3691,12 @@
         <f t="shared" si="1"/>
         <v>97.50238095</v>
       </c>
+      <c r="D10" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="10">
+      <c r="A11" s="11">
         <v>61.0</v>
       </c>
       <c r="B11" s="4">
@@ -3363,6 +3705,9 @@
       <c r="C11" s="7">
         <f t="shared" si="1"/>
         <v>97.35238095</v>
+      </c>
+      <c r="D11" s="3">
+        <v>99.0</v>
       </c>
     </row>
     <row r="12">
@@ -3376,6 +3721,9 @@
         <f t="shared" si="1"/>
         <v>97.10238095</v>
       </c>
+      <c r="D12" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -3388,6 +3736,9 @@
         <f t="shared" si="1"/>
         <v>96.90238095</v>
       </c>
+      <c r="D13" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -3400,6 +3751,9 @@
         <f t="shared" si="1"/>
         <v>96.60238095</v>
       </c>
+      <c r="D14" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -3412,6 +3766,9 @@
         <f t="shared" si="1"/>
         <v>95.66331429</v>
       </c>
+      <c r="D15" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -3424,6 +3781,9 @@
         <f t="shared" si="1"/>
         <v>94.73333333</v>
       </c>
+      <c r="D16" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -3436,6 +3796,9 @@
         <f t="shared" si="1"/>
         <v>93.02380952</v>
       </c>
+      <c r="D17" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -3448,6 +3811,9 @@
         <f t="shared" si="1"/>
         <v>91.31428571</v>
       </c>
+      <c r="D18" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -3460,6 +3826,9 @@
         <f t="shared" si="1"/>
         <v>89.6047619</v>
       </c>
+      <c r="D19" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -3472,6 +3841,9 @@
         <f t="shared" si="1"/>
         <v>87.8952381</v>
       </c>
+      <c r="D20" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -3484,6 +3856,9 @@
         <f t="shared" si="1"/>
         <v>86.18571429</v>
       </c>
+      <c r="D21" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -3496,6 +3871,9 @@
         <f t="shared" si="1"/>
         <v>84.47619048</v>
       </c>
+      <c r="D22" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -3508,6 +3886,9 @@
         <f t="shared" si="1"/>
         <v>82.76666667</v>
       </c>
+      <c r="D23" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
@@ -3520,6 +3901,9 @@
         <f t="shared" si="1"/>
         <v>81.05714286</v>
       </c>
+      <c r="D24" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
@@ -3532,6 +3916,9 @@
         <f t="shared" si="1"/>
         <v>79.34761905</v>
       </c>
+      <c r="D25" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
@@ -3544,6 +3931,9 @@
         <f t="shared" si="1"/>
         <v>77.63809524</v>
       </c>
+      <c r="D26" s="3">
+        <v>99.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -3556,6 +3946,9 @@
         <f t="shared" si="1"/>
         <v>75.92857143</v>
       </c>
+      <c r="D27" s="3">
+        <v>98.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
@@ -3568,6 +3961,9 @@
         <f t="shared" si="1"/>
         <v>74.21904762</v>
       </c>
+      <c r="D28" s="3">
+        <v>96.7999999999999</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
@@ -3580,6 +3976,9 @@
         <f t="shared" si="1"/>
         <v>72.50952381</v>
       </c>
+      <c r="D29" s="3">
+        <v>94.5999999999999</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
@@ -3592,6 +3991,9 @@
         <f t="shared" si="1"/>
         <v>70.8</v>
       </c>
+      <c r="D30" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
@@ -3604,6 +4006,9 @@
         <f t="shared" si="1"/>
         <v>69.09047619</v>
       </c>
+      <c r="D31" s="3">
+        <v>90.2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
@@ -3616,6 +4021,9 @@
         <f t="shared" si="1"/>
         <v>67.38095238</v>
       </c>
+      <c r="D32" s="3">
+        <v>88.0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
@@ -3628,6 +4036,9 @@
         <f t="shared" si="1"/>
         <v>65.67142857</v>
       </c>
+      <c r="D33" s="3">
+        <v>85.8</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
@@ -3640,6 +4051,9 @@
         <f t="shared" si="1"/>
         <v>63.96190476</v>
       </c>
+      <c r="D34" s="3">
+        <v>83.6</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
@@ -3652,6 +4066,9 @@
         <f t="shared" si="1"/>
         <v>62.25238095</v>
       </c>
+      <c r="D35" s="3">
+        <v>81.4</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
@@ -3664,6 +4081,9 @@
         <f t="shared" si="1"/>
         <v>60.54285714</v>
       </c>
+      <c r="D36" s="3">
+        <v>79.2</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
@@ -3676,6 +4096,9 @@
         <f t="shared" si="1"/>
         <v>58.83333333</v>
       </c>
+      <c r="D37" s="3">
+        <v>77.0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
@@ -3688,6 +4111,9 @@
         <f t="shared" si="1"/>
         <v>57.12380952</v>
       </c>
+      <c r="D38" s="3">
+        <v>74.8</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
@@ -3700,6 +4126,9 @@
         <f t="shared" si="1"/>
         <v>55.41428571</v>
       </c>
+      <c r="D39" s="3">
+        <v>72.6</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
@@ -3712,6 +4141,9 @@
         <f t="shared" si="1"/>
         <v>53.7047619</v>
       </c>
+      <c r="D40" s="3">
+        <v>70.4</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
@@ -3724,6 +4156,9 @@
         <f t="shared" si="1"/>
         <v>51.9952381</v>
       </c>
+      <c r="D41" s="3">
+        <v>68.2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
@@ -3736,6 +4171,9 @@
         <f t="shared" si="1"/>
         <v>50.28571429</v>
       </c>
+      <c r="D42" s="3">
+        <v>66.0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
@@ -3748,6 +4186,9 @@
         <f t="shared" si="1"/>
         <v>48.57619048</v>
       </c>
+      <c r="D43" s="3">
+        <v>63.8</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
@@ -3760,6 +4201,9 @@
         <f t="shared" si="1"/>
         <v>46.86666667</v>
       </c>
+      <c r="D44" s="3">
+        <v>61.6</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
@@ -3772,6 +4216,9 @@
         <f t="shared" si="1"/>
         <v>45.15714286</v>
       </c>
+      <c r="D45" s="3">
+        <v>59.4</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
@@ -3784,6 +4231,9 @@
         <f t="shared" si="1"/>
         <v>43.44761905</v>
       </c>
+      <c r="D46" s="3">
+        <v>57.2</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
@@ -3796,6 +4246,9 @@
         <f t="shared" si="1"/>
         <v>41.73809524</v>
       </c>
+      <c r="D47" s="3">
+        <v>55.0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
@@ -3808,6 +4261,9 @@
         <f t="shared" si="1"/>
         <v>40.02857143</v>
       </c>
+      <c r="D48" s="3">
+        <v>52.8</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
@@ -3820,6 +4276,9 @@
         <f t="shared" si="1"/>
         <v>38.31904762</v>
       </c>
+      <c r="D49" s="3">
+        <v>50.6</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
@@ -3832,6 +4291,9 @@
         <f t="shared" si="1"/>
         <v>36.60952381</v>
       </c>
+      <c r="D50" s="3">
+        <v>48.4</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
@@ -3844,6 +4306,9 @@
         <f t="shared" si="1"/>
         <v>34.9</v>
       </c>
+      <c r="D51" s="3">
+        <v>46.2</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
@@ -3856,6 +4321,9 @@
         <f t="shared" si="1"/>
         <v>33.19047619</v>
       </c>
+      <c r="D52" s="3">
+        <v>44.0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
@@ -3868,6 +4336,9 @@
         <f t="shared" si="1"/>
         <v>31.48095238</v>
       </c>
+      <c r="D53" s="3">
+        <v>41.8</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
@@ -3880,6 +4351,9 @@
         <f t="shared" si="1"/>
         <v>29.77142857</v>
       </c>
+      <c r="D54" s="3">
+        <v>39.6</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
@@ -3892,6 +4366,9 @@
         <f t="shared" si="1"/>
         <v>28.06190476</v>
       </c>
+      <c r="D55" s="3">
+        <v>37.4</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
@@ -3904,6 +4381,9 @@
         <f t="shared" si="1"/>
         <v>26.35238095</v>
       </c>
+      <c r="D56" s="3">
+        <v>35.2</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
@@ -3916,6 +4396,9 @@
         <f t="shared" si="1"/>
         <v>24.64285714</v>
       </c>
+      <c r="D57" s="3">
+        <v>33.0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
@@ -3928,6 +4411,9 @@
         <f t="shared" si="1"/>
         <v>22.93333333</v>
       </c>
+      <c r="D58" s="3">
+        <v>30.8</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
@@ -3940,6 +4426,9 @@
         <f t="shared" si="1"/>
         <v>21.22380952</v>
       </c>
+      <c r="D59" s="3">
+        <v>28.6</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
@@ -3952,6 +4441,9 @@
         <f t="shared" si="1"/>
         <v>19.51428571</v>
       </c>
+      <c r="D60" s="3">
+        <v>26.4</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
@@ -3964,6 +4456,9 @@
         <f t="shared" si="1"/>
         <v>17.8047619</v>
       </c>
+      <c r="D61" s="3">
+        <v>24.2</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
@@ -3976,6 +4471,9 @@
         <f t="shared" si="1"/>
         <v>16.0952381</v>
       </c>
+      <c r="D62" s="3">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
@@ -3988,6 +4486,9 @@
         <f t="shared" si="1"/>
         <v>14.38571429</v>
       </c>
+      <c r="D63" s="3">
+        <v>19.8</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
@@ -4000,6 +4501,9 @@
         <f t="shared" si="1"/>
         <v>12.67619048</v>
       </c>
+      <c r="D64" s="3">
+        <v>17.6</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
@@ -4012,6 +4516,9 @@
         <f t="shared" si="1"/>
         <v>10.96666667</v>
       </c>
+      <c r="D65" s="3">
+        <v>15.4</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
@@ -4024,6 +4531,9 @@
         <f t="shared" si="1"/>
         <v>9.257142857</v>
       </c>
+      <c r="D66" s="3">
+        <v>13.2</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
@@ -4036,6 +4546,9 @@
         <f t="shared" si="1"/>
         <v>7.547619048</v>
       </c>
+      <c r="D67" s="3">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
@@ -4048,6 +4561,9 @@
         <f t="shared" si="1"/>
         <v>5.838095238</v>
       </c>
+      <c r="D68" s="3">
+        <v>8.8</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
@@ -4060,6 +4576,9 @@
         <f t="shared" si="1"/>
         <v>4.128571429</v>
       </c>
+      <c r="D69" s="3">
+        <v>6.6</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
@@ -4072,6 +4591,9 @@
         <f t="shared" si="1"/>
         <v>2.419047619</v>
       </c>
+      <c r="D70" s="3">
+        <v>4.4</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
@@ -4084,6 +4606,9 @@
         <f t="shared" si="1"/>
         <v>0.7095238095</v>
       </c>
+      <c r="D71" s="3">
+        <v>2.2</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="3">
@@ -4095,6 +4620,9 @@
       <c r="C72" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
+      </c>
+      <c r="D72" s="3">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -4121,10 +4649,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">

</xml_diff>